<commit_message>
backup final before zhilyakov fixes
</commit_message>
<xml_diff>
--- a/images/AcuiringDatasetSplit.xlsx
+++ b/images/AcuiringDatasetSplit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YandexDisk\Документы\Аспирантура документы\Russian-Phd-LaTeX-Dissertation-Template-master\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76542D51-EAD4-4C33-9210-7E2E6FFB5F94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACA188F-AB94-4B1C-8933-D27F73DDFA92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{747752B2-6BBA-4D31-A9A7-282C05BD9CBA}"/>
   </bookViews>
@@ -36,19 +36,22 @@
     <t>…</t>
   </si>
   <si>
-    <t>Номер ряда</t>
+    <t>обучающий диапазон</t>
   </si>
   <si>
-    <t>тренировочный период</t>
+    <t>тестовый диапазон</t>
   </si>
   <si>
-    <t>тестовый период</t>
+    <t>Номер временного ряда</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/yyyy"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,7 +129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -279,19 +282,6 @@
       <right/>
       <top style="medium">
         <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color auto="1"/>
-      </left>
-      <right style="dotted">
-        <color auto="1"/>
-      </right>
-      <top style="dotted">
-        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -324,21 +314,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" textRotation="90"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
@@ -356,9 +337,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -369,29 +347,38 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" textRotation="90"/>
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -421,8 +408,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>184148</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>452</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>158751</xdr:rowOff>
     </xdr:from>
@@ -445,8 +432,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="2136773" y="3038476"/>
-          <a:ext cx="203200" cy="1111249"/>
+          <a:off x="2024741" y="3046641"/>
+          <a:ext cx="202746" cy="1108074"/>
         </a:xfrm>
         <a:prstGeom prst="rightBrace">
           <a:avLst/>
@@ -479,13 +466,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
@@ -503,8 +490,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1720850" y="3683000"/>
-          <a:ext cx="1009650" cy="260350"/>
+          <a:off x="1428750" y="3683000"/>
+          <a:ext cx="1377950" cy="260350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -541,17 +528,151 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="ru-RU" sz="1100"/>
-            <a:t>лаговое</a:t>
+            <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
+            <a:t>окно</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
-            <a:t> окно</a:t>
+            <a:t>запаздывания</a:t>
           </a:r>
           <a:endParaRPr lang="ru-RU" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>30080</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>187158</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>78537</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66173</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59E7D3A5-7273-4D7D-A3F6-B8A2B97F4AC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2523291" y="2944395"/>
+          <a:ext cx="2070430" cy="260015"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF">
+            <a:alpha val="32941"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:softEdge rad="31750"/>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
+            <a:t>окно прогнозирования при </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>h=1</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>106950</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>43447</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>40105</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>90237</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEBB6A77-AE8B-49E5-94A2-33CA2EDCBC64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2783976" y="3181684"/>
+          <a:ext cx="300787" cy="237290"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -856,562 +977,563 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED80AE5F-AE02-412C-BBB7-7CBA6B8DA430}">
   <dimension ref="C1:AO26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15:AB15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="2.6328125" customWidth="1"/>
     <col min="3" max="3" width="2.54296875" customWidth="1"/>
-    <col min="4" max="4" width="7.36328125" customWidth="1"/>
+    <col min="4" max="4" width="8.08984375" customWidth="1"/>
     <col min="5" max="5" width="2.08984375" customWidth="1"/>
     <col min="6" max="41" width="2.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:41" x14ac:dyDescent="0.35">
-      <c r="AD1" s="7"/>
+      <c r="AD1" s="4"/>
     </row>
     <row r="2" spans="4:41" x14ac:dyDescent="0.35">
-      <c r="AD2" s="7"/>
+      <c r="AD2" s="4"/>
     </row>
     <row r="3" spans="4:41" x14ac:dyDescent="0.35">
-      <c r="AD3" s="7"/>
+      <c r="AD3" s="4"/>
     </row>
     <row r="4" spans="4:41" x14ac:dyDescent="0.35">
-      <c r="AD4" s="7"/>
+      <c r="AD4" s="4"/>
     </row>
     <row r="5" spans="4:41" x14ac:dyDescent="0.35">
-      <c r="AD5" s="7"/>
+      <c r="AD5" s="4"/>
     </row>
     <row r="6" spans="4:41" x14ac:dyDescent="0.35">
-      <c r="AD6" s="7"/>
+      <c r="AD6" s="4"/>
     </row>
     <row r="7" spans="4:41" x14ac:dyDescent="0.35">
-      <c r="AD7" s="7"/>
+      <c r="AD7" s="4"/>
     </row>
     <row r="8" spans="4:41" x14ac:dyDescent="0.35">
-      <c r="AD8" s="7"/>
+      <c r="AD8" s="4"/>
     </row>
     <row r="9" spans="4:41" x14ac:dyDescent="0.35">
-      <c r="AD9" s="7"/>
+      <c r="AD9" s="4"/>
     </row>
     <row r="10" spans="4:41" x14ac:dyDescent="0.35">
-      <c r="AD10" s="7"/>
+      <c r="AD10" s="4"/>
     </row>
     <row r="11" spans="4:41" x14ac:dyDescent="0.35">
-      <c r="AD11" s="7"/>
+      <c r="AD11" s="4"/>
     </row>
     <row r="12" spans="4:41" x14ac:dyDescent="0.35">
-      <c r="AD12" s="7"/>
+      <c r="AD12" s="4"/>
     </row>
     <row r="13" spans="4:41" x14ac:dyDescent="0.35">
-      <c r="AD13" s="7"/>
+      <c r="AD13" s="4"/>
     </row>
     <row r="14" spans="4:41" x14ac:dyDescent="0.35">
-      <c r="AD14" s="7"/>
-    </row>
-    <row r="15" spans="4:41" x14ac:dyDescent="0.35">
-      <c r="D15" s="34" t="s">
+      <c r="D14" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD14" s="4"/>
+    </row>
+    <row r="15" spans="4:41" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="38"/>
+      <c r="H15" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="38" t="s">
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="S15" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="38"/>
-      <c r="P15" s="38"/>
-      <c r="S15" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="T15" s="39"/>
-      <c r="U15" s="39"/>
-      <c r="V15" s="39"/>
-      <c r="W15" s="39"/>
-      <c r="X15" s="39"/>
-      <c r="Y15" s="39"/>
-      <c r="Z15" s="39"/>
-      <c r="AA15" s="39"/>
-      <c r="AB15" s="39"/>
-      <c r="AD15" s="7"/>
+      <c r="T15" s="37"/>
+      <c r="U15" s="37"/>
+      <c r="V15" s="37"/>
+      <c r="W15" s="37"/>
+      <c r="X15" s="37"/>
+      <c r="Y15" s="37"/>
+      <c r="Z15" s="37"/>
+      <c r="AA15" s="37"/>
+      <c r="AB15" s="37"/>
+      <c r="AD15" s="4"/>
     </row>
     <row r="16" spans="4:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D16" s="35"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="7"/>
-      <c r="Z16" s="7"/>
-      <c r="AA16" s="7"/>
-      <c r="AB16" s="7"/>
-      <c r="AC16" s="7"/>
-      <c r="AD16" s="3"/>
-      <c r="AE16" s="10"/>
-      <c r="AF16" s="10"/>
-      <c r="AG16" s="10"/>
-      <c r="AH16" s="10"/>
-      <c r="AI16" s="10"/>
-      <c r="AJ16" s="10"/>
-      <c r="AK16" s="10"/>
-      <c r="AL16" s="10"/>
-      <c r="AM16" s="10"/>
-      <c r="AN16" s="10"/>
-      <c r="AO16" s="10"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="4"/>
+      <c r="AB16" s="4"/>
+      <c r="AC16" s="4"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="7"/>
+      <c r="AG16" s="7"/>
+      <c r="AH16" s="7"/>
+      <c r="AI16" s="7"/>
+      <c r="AJ16" s="7"/>
+      <c r="AK16" s="7"/>
+      <c r="AL16" s="7"/>
+      <c r="AM16" s="7"/>
+      <c r="AN16" s="7"/>
+      <c r="AO16" s="7"/>
     </row>
     <row r="17" spans="3:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D17" s="33">
+      <c r="D17" s="28">
         <v>1</v>
       </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="13"/>
-      <c r="W17" s="13"/>
-      <c r="X17" s="22"/>
-      <c r="Y17" s="23"/>
-      <c r="Z17" s="23"/>
-      <c r="AA17" s="23"/>
-      <c r="AB17" s="23"/>
-      <c r="AC17" s="23"/>
-      <c r="AD17" s="24"/>
-      <c r="AE17" s="11"/>
-      <c r="AF17" s="11"/>
-      <c r="AG17" s="11"/>
-      <c r="AH17" s="11"/>
-      <c r="AI17" s="11"/>
-      <c r="AJ17" s="11"/>
-      <c r="AK17" s="11"/>
-      <c r="AL17" s="11"/>
-      <c r="AM17" s="11"/>
-      <c r="AN17" s="11"/>
-      <c r="AO17" s="11"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="18"/>
+      <c r="Y17" s="19"/>
+      <c r="Z17" s="19"/>
+      <c r="AA17" s="19"/>
+      <c r="AB17" s="19"/>
+      <c r="AC17" s="19"/>
+      <c r="AD17" s="20"/>
+      <c r="AE17" s="8"/>
+      <c r="AF17" s="8"/>
+      <c r="AG17" s="8"/>
+      <c r="AH17" s="8"/>
+      <c r="AI17" s="8"/>
+      <c r="AJ17" s="8"/>
+      <c r="AK17" s="8"/>
+      <c r="AL17" s="8"/>
+      <c r="AM17" s="8"/>
+      <c r="AN17" s="8"/>
+      <c r="AO17" s="8"/>
     </row>
     <row r="18" spans="3:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D18" s="33"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
-      <c r="W18" s="13"/>
-      <c r="X18" s="22"/>
-      <c r="Y18" s="23"/>
-      <c r="Z18" s="23"/>
-      <c r="AA18" s="23"/>
-      <c r="AB18" s="23"/>
-      <c r="AC18" s="23"/>
-      <c r="AD18" s="24"/>
-      <c r="AE18" s="11"/>
-      <c r="AF18" s="11"/>
-      <c r="AG18" s="11"/>
-      <c r="AH18" s="11"/>
-      <c r="AI18" s="11"/>
-      <c r="AJ18" s="11"/>
-      <c r="AK18" s="11"/>
-      <c r="AL18" s="11"/>
-      <c r="AM18" s="11"/>
-      <c r="AN18" s="11"/>
-      <c r="AO18" s="11"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="18"/>
+      <c r="Y18" s="19"/>
+      <c r="Z18" s="19"/>
+      <c r="AA18" s="19"/>
+      <c r="AB18" s="19"/>
+      <c r="AC18" s="19"/>
+      <c r="AD18" s="20"/>
+      <c r="AE18" s="8"/>
+      <c r="AF18" s="8"/>
+      <c r="AG18" s="8"/>
+      <c r="AH18" s="8"/>
+      <c r="AI18" s="8"/>
+      <c r="AJ18" s="8"/>
+      <c r="AK18" s="8"/>
+      <c r="AL18" s="8"/>
+      <c r="AM18" s="8"/>
+      <c r="AN18" s="8"/>
+      <c r="AO18" s="8"/>
     </row>
     <row r="19" spans="3:41" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="D19" s="33"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="14"/>
-      <c r="W19" s="14"/>
-      <c r="X19" s="22"/>
-      <c r="Y19" s="23"/>
-      <c r="Z19" s="23"/>
-      <c r="AA19" s="23"/>
-      <c r="AB19" s="23"/>
-      <c r="AC19" s="23"/>
-      <c r="AD19" s="25"/>
-      <c r="AE19" s="12"/>
-      <c r="AF19" s="12"/>
-      <c r="AG19" s="12"/>
-      <c r="AH19" s="12"/>
-      <c r="AI19" s="12"/>
-      <c r="AJ19" s="12"/>
-      <c r="AK19" s="12"/>
-      <c r="AL19" s="12"/>
-      <c r="AM19" s="12"/>
-      <c r="AN19" s="12"/>
-      <c r="AO19" s="12"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="18"/>
+      <c r="Y19" s="19"/>
+      <c r="Z19" s="19"/>
+      <c r="AA19" s="19"/>
+      <c r="AB19" s="19"/>
+      <c r="AC19" s="19"/>
+      <c r="AD19" s="21"/>
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="9"/>
+      <c r="AG19" s="9"/>
+      <c r="AH19" s="9"/>
+      <c r="AI19" s="9"/>
+      <c r="AJ19" s="9"/>
+      <c r="AK19" s="9"/>
+      <c r="AL19" s="9"/>
+      <c r="AM19" s="9"/>
+      <c r="AN19" s="9"/>
+      <c r="AO19" s="9"/>
     </row>
     <row r="20" spans="3:41" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="D20" s="33"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="21" t="s">
+      <c r="D20" s="28"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="21"/>
-      <c r="X20" s="26"/>
-      <c r="Y20" s="27"/>
-      <c r="Z20" s="27"/>
-      <c r="AA20" s="27"/>
-      <c r="AB20" s="27"/>
-      <c r="AC20" s="27"/>
-      <c r="AD20" s="24"/>
-      <c r="AE20" s="11"/>
-      <c r="AF20" s="11"/>
-      <c r="AG20" s="11"/>
-      <c r="AH20" s="11"/>
-      <c r="AI20" s="11"/>
-      <c r="AJ20" s="11"/>
-      <c r="AK20" s="11"/>
-      <c r="AL20" s="11"/>
-      <c r="AM20" s="11"/>
-      <c r="AN20" s="11"/>
-      <c r="AO20" s="11"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="35"/>
+      <c r="S20" s="35"/>
+      <c r="T20" s="35"/>
+      <c r="U20" s="35"/>
+      <c r="V20" s="35"/>
+      <c r="W20" s="35"/>
+      <c r="X20" s="22"/>
+      <c r="Y20" s="23"/>
+      <c r="Z20" s="23"/>
+      <c r="AA20" s="23"/>
+      <c r="AB20" s="23"/>
+      <c r="AC20" s="23"/>
+      <c r="AD20" s="20"/>
+      <c r="AE20" s="8"/>
+      <c r="AF20" s="8"/>
+      <c r="AG20" s="8"/>
+      <c r="AH20" s="8"/>
+      <c r="AI20" s="8"/>
+      <c r="AJ20" s="8"/>
+      <c r="AK20" s="8"/>
+      <c r="AL20" s="8"/>
+      <c r="AM20" s="8"/>
+      <c r="AN20" s="8"/>
+      <c r="AO20" s="8"/>
     </row>
     <row r="21" spans="3:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="4"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18"/>
-      <c r="T21" s="18"/>
-      <c r="U21" s="18"/>
-      <c r="V21" s="19"/>
-      <c r="W21" s="20"/>
-      <c r="X21" s="22"/>
-      <c r="Y21" s="23"/>
-      <c r="Z21" s="23"/>
-      <c r="AA21" s="23"/>
-      <c r="AB21" s="23"/>
-      <c r="AC21" s="23"/>
-      <c r="AD21" s="28"/>
-      <c r="AE21" s="30"/>
-      <c r="AF21" s="9"/>
-      <c r="AG21" s="9"/>
-      <c r="AH21" s="11"/>
-      <c r="AI21" s="11"/>
-      <c r="AJ21" s="11"/>
-      <c r="AK21" s="11"/>
-      <c r="AL21" s="11"/>
-      <c r="AM21" s="11"/>
-      <c r="AN21" s="11"/>
-      <c r="AO21" s="11"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="16"/>
+      <c r="W21" s="17"/>
+      <c r="X21" s="18"/>
+      <c r="Y21" s="19"/>
+      <c r="Z21" s="19"/>
+      <c r="AA21" s="19"/>
+      <c r="AB21" s="19"/>
+      <c r="AC21" s="19"/>
+      <c r="AD21" s="24"/>
+      <c r="AE21" s="26"/>
+      <c r="AF21" s="6"/>
+      <c r="AG21" s="6"/>
+      <c r="AH21" s="8"/>
+      <c r="AI21" s="8"/>
+      <c r="AJ21" s="8"/>
+      <c r="AK21" s="8"/>
+      <c r="AL21" s="8"/>
+      <c r="AM21" s="8"/>
+      <c r="AN21" s="8"/>
+      <c r="AO21" s="8"/>
     </row>
     <row r="22" spans="3:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C22" s="4"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
-      <c r="T22" s="18"/>
-      <c r="U22" s="18"/>
-      <c r="V22" s="18"/>
-      <c r="W22" s="19"/>
-      <c r="X22" s="22"/>
-      <c r="Y22" s="23"/>
-      <c r="Z22" s="23"/>
-      <c r="AA22" s="23"/>
-      <c r="AB22" s="23"/>
-      <c r="AC22" s="23"/>
-      <c r="AD22" s="28"/>
-      <c r="AE22" s="30"/>
-      <c r="AF22" s="9"/>
-      <c r="AG22" s="9"/>
-      <c r="AH22" s="11"/>
-      <c r="AI22" s="11"/>
-      <c r="AJ22" s="11"/>
-      <c r="AK22" s="11"/>
-      <c r="AL22" s="11"/>
-      <c r="AM22" s="11"/>
-      <c r="AN22" s="11"/>
-      <c r="AO22" s="11"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="16"/>
+      <c r="X22" s="18"/>
+      <c r="Y22" s="19"/>
+      <c r="Z22" s="19"/>
+      <c r="AA22" s="19"/>
+      <c r="AB22" s="19"/>
+      <c r="AC22" s="19"/>
+      <c r="AD22" s="24"/>
+      <c r="AE22" s="26"/>
+      <c r="AF22" s="6"/>
+      <c r="AG22" s="6"/>
+      <c r="AH22" s="8"/>
+      <c r="AI22" s="8"/>
+      <c r="AJ22" s="8"/>
+      <c r="AK22" s="8"/>
+      <c r="AL22" s="8"/>
+      <c r="AM22" s="8"/>
+      <c r="AN22" s="8"/>
+      <c r="AO22" s="8"/>
     </row>
     <row r="23" spans="3:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C23" s="4"/>
-      <c r="D23" s="36">
+      <c r="C23" s="34"/>
+      <c r="D23" s="29">
         <v>1731</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="16"/>
-      <c r="T23" s="16"/>
-      <c r="U23" s="16"/>
-      <c r="V23" s="16"/>
-      <c r="W23" s="16"/>
-      <c r="X23" s="29"/>
-      <c r="Y23" s="23"/>
-      <c r="Z23" s="23"/>
-      <c r="AA23" s="23"/>
-      <c r="AB23" s="23"/>
-      <c r="AC23" s="23"/>
-      <c r="AD23" s="28"/>
-      <c r="AE23" s="30"/>
-      <c r="AF23" s="9"/>
-      <c r="AG23" s="9"/>
-      <c r="AH23" s="11"/>
-      <c r="AI23" s="11"/>
-      <c r="AJ23" s="11"/>
-      <c r="AK23" s="11"/>
-      <c r="AL23" s="11"/>
-      <c r="AM23" s="11"/>
-      <c r="AN23" s="11"/>
-      <c r="AO23" s="11"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13"/>
+      <c r="W23" s="13"/>
+      <c r="X23" s="25"/>
+      <c r="Y23" s="19"/>
+      <c r="Z23" s="19"/>
+      <c r="AA23" s="19"/>
+      <c r="AB23" s="19"/>
+      <c r="AC23" s="19"/>
+      <c r="AD23" s="24"/>
+      <c r="AE23" s="26"/>
+      <c r="AF23" s="6"/>
+      <c r="AG23" s="6"/>
+      <c r="AH23" s="8"/>
+      <c r="AI23" s="8"/>
+      <c r="AJ23" s="8"/>
+      <c r="AK23" s="8"/>
+      <c r="AL23" s="8"/>
+      <c r="AM23" s="8"/>
+      <c r="AN23" s="8"/>
+      <c r="AO23" s="8"/>
     </row>
     <row r="24" spans="3:41" ht="9.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="AD24" s="37"/>
+      <c r="AD24" s="30"/>
     </row>
     <row r="25" spans="3:41" ht="81" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F25" s="2">
+      <c r="F25" s="31">
         <v>44197</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="32">
         <f t="shared" ref="G25:AO25" si="0">EOMONTH(G26, 0)</f>
         <v>44255</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25" s="32">
         <f t="shared" si="0"/>
         <v>44286</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="32">
         <f t="shared" si="0"/>
         <v>44316</v>
       </c>
-      <c r="J25" s="5">
+      <c r="J25" s="32">
         <f t="shared" si="0"/>
         <v>44347</v>
       </c>
-      <c r="K25" s="5">
+      <c r="K25" s="32">
         <f t="shared" si="0"/>
         <v>44377</v>
       </c>
-      <c r="L25" s="5">
+      <c r="L25" s="32">
         <f t="shared" si="0"/>
         <v>44408</v>
       </c>
-      <c r="M25" s="5">
+      <c r="M25" s="32">
         <f t="shared" si="0"/>
         <v>44439</v>
       </c>
-      <c r="N25" s="5">
+      <c r="N25" s="32">
         <f t="shared" si="0"/>
         <v>44469</v>
       </c>
-      <c r="O25" s="5">
+      <c r="O25" s="32">
         <f t="shared" si="0"/>
         <v>44500</v>
       </c>
-      <c r="P25" s="5">
+      <c r="P25" s="32">
         <f t="shared" si="0"/>
         <v>44530</v>
       </c>
-      <c r="Q25" s="5">
+      <c r="Q25" s="32">
         <f t="shared" si="0"/>
         <v>44561</v>
       </c>
-      <c r="R25" s="5">
+      <c r="R25" s="32">
         <f t="shared" si="0"/>
         <v>44592</v>
       </c>
-      <c r="S25" s="5">
+      <c r="S25" s="32">
         <f t="shared" si="0"/>
         <v>44620</v>
       </c>
-      <c r="T25" s="5">
+      <c r="T25" s="32">
         <f t="shared" si="0"/>
         <v>44651</v>
       </c>
-      <c r="U25" s="5">
+      <c r="U25" s="32">
         <f t="shared" si="0"/>
         <v>44681</v>
       </c>
-      <c r="V25" s="5">
+      <c r="V25" s="32">
         <f t="shared" si="0"/>
         <v>44712</v>
       </c>
-      <c r="W25" s="5">
+      <c r="W25" s="32">
         <f t="shared" si="0"/>
         <v>44742</v>
       </c>
-      <c r="X25" s="5">
+      <c r="X25" s="32">
         <f t="shared" si="0"/>
         <v>44773</v>
       </c>
-      <c r="Y25" s="5">
+      <c r="Y25" s="32">
         <f t="shared" si="0"/>
         <v>44804</v>
       </c>
-      <c r="Z25" s="5">
+      <c r="Z25" s="32">
         <f t="shared" si="0"/>
         <v>44834</v>
       </c>
-      <c r="AA25" s="5">
+      <c r="AA25" s="32">
         <f t="shared" si="0"/>
         <v>44865</v>
       </c>
-      <c r="AB25" s="5">
+      <c r="AB25" s="32">
         <f t="shared" si="0"/>
         <v>44895</v>
       </c>
-      <c r="AC25" s="2">
+      <c r="AC25" s="31">
         <f t="shared" si="0"/>
         <v>44926</v>
       </c>
-      <c r="AD25" s="31">
+      <c r="AD25" s="33">
         <v>44927</v>
       </c>
-      <c r="AE25" s="5">
+      <c r="AE25" s="32">
         <f t="shared" si="0"/>
         <v>44985</v>
       </c>
-      <c r="AF25" s="5">
+      <c r="AF25" s="32">
         <f t="shared" si="0"/>
         <v>45016</v>
       </c>
-      <c r="AG25" s="5">
+      <c r="AG25" s="32">
         <f t="shared" si="0"/>
         <v>45046</v>
       </c>
-      <c r="AH25" s="5">
+      <c r="AH25" s="32">
         <f t="shared" si="0"/>
         <v>45077</v>
       </c>
-      <c r="AI25" s="5">
+      <c r="AI25" s="32">
         <f t="shared" si="0"/>
         <v>45107</v>
       </c>
-      <c r="AJ25" s="5">
+      <c r="AJ25" s="32">
         <f t="shared" si="0"/>
         <v>45138</v>
       </c>
-      <c r="AK25" s="5">
+      <c r="AK25" s="32">
         <f t="shared" si="0"/>
         <v>45169</v>
       </c>
-      <c r="AL25" s="5">
+      <c r="AL25" s="32">
         <f t="shared" si="0"/>
         <v>45199</v>
       </c>
-      <c r="AM25" s="5">
+      <c r="AM25" s="32">
         <f t="shared" si="0"/>
         <v>45230</v>
       </c>
-      <c r="AN25" s="5">
+      <c r="AN25" s="32">
         <f t="shared" si="0"/>
         <v>45260</v>
       </c>
-      <c r="AO25" s="2">
+      <c r="AO25" s="31">
         <f t="shared" si="0"/>
         <v>45291</v>
       </c>
@@ -1420,106 +1542,106 @@
       <c r="F26" s="1">
         <v>44197</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="3">
         <v>44228</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H26" s="3">
         <v>44256</v>
       </c>
-      <c r="I26" s="6">
+      <c r="I26" s="3">
         <v>44287</v>
       </c>
-      <c r="J26" s="6">
+      <c r="J26" s="3">
         <v>44317</v>
       </c>
-      <c r="K26" s="6">
+      <c r="K26" s="3">
         <v>44348</v>
       </c>
-      <c r="L26" s="6">
+      <c r="L26" s="3">
         <v>44378</v>
       </c>
-      <c r="M26" s="6">
+      <c r="M26" s="3">
         <v>44409</v>
       </c>
-      <c r="N26" s="6">
+      <c r="N26" s="3">
         <v>44440</v>
       </c>
-      <c r="O26" s="6">
+      <c r="O26" s="3">
         <v>44470</v>
       </c>
-      <c r="P26" s="6">
+      <c r="P26" s="3">
         <v>44501</v>
       </c>
-      <c r="Q26" s="6">
+      <c r="Q26" s="3">
         <v>44531</v>
       </c>
-      <c r="R26" s="6">
+      <c r="R26" s="3">
         <v>44562</v>
       </c>
-      <c r="S26" s="6">
+      <c r="S26" s="3">
         <v>44593</v>
       </c>
-      <c r="T26" s="6">
+      <c r="T26" s="3">
         <v>44621</v>
       </c>
-      <c r="U26" s="6">
+      <c r="U26" s="3">
         <v>44652</v>
       </c>
-      <c r="V26" s="6">
+      <c r="V26" s="3">
         <v>44682</v>
       </c>
-      <c r="W26" s="6">
+      <c r="W26" s="3">
         <v>44713</v>
       </c>
-      <c r="X26" s="6">
+      <c r="X26" s="3">
         <v>44743</v>
       </c>
-      <c r="Y26" s="6">
+      <c r="Y26" s="3">
         <v>44774</v>
       </c>
-      <c r="Z26" s="6">
+      <c r="Z26" s="3">
         <v>44805</v>
       </c>
-      <c r="AA26" s="6">
+      <c r="AA26" s="3">
         <v>44835</v>
       </c>
-      <c r="AB26" s="6">
+      <c r="AB26" s="3">
         <v>44866</v>
       </c>
       <c r="AC26" s="1">
         <v>44896</v>
       </c>
-      <c r="AD26" s="32">
+      <c r="AD26" s="27">
         <v>44927</v>
       </c>
-      <c r="AE26" s="6">
+      <c r="AE26" s="3">
         <v>44958</v>
       </c>
-      <c r="AF26" s="6">
+      <c r="AF26" s="3">
         <v>44986</v>
       </c>
-      <c r="AG26" s="6">
+      <c r="AG26" s="3">
         <v>45017</v>
       </c>
-      <c r="AH26" s="6">
+      <c r="AH26" s="3">
         <v>45047</v>
       </c>
-      <c r="AI26" s="6">
+      <c r="AI26" s="3">
         <v>45078</v>
       </c>
-      <c r="AJ26" s="6">
+      <c r="AJ26" s="3">
         <v>45108</v>
       </c>
-      <c r="AK26" s="6">
+      <c r="AK26" s="3">
         <v>45139</v>
       </c>
-      <c r="AL26" s="6">
+      <c r="AL26" s="3">
         <v>45170</v>
       </c>
-      <c r="AM26" s="6">
+      <c r="AM26" s="3">
         <v>45200</v>
       </c>
-      <c r="AN26" s="6">
+      <c r="AN26" s="3">
         <v>45231</v>
       </c>
       <c r="AO26" s="1">
@@ -1530,9 +1652,9 @@
   <mergeCells count="5">
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="F20:W20"/>
-    <mergeCell ref="D15:D16"/>
     <mergeCell ref="H15:P15"/>
     <mergeCell ref="S15:AB15"/>
+    <mergeCell ref="D14:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>